<commit_message>
Add new calculation for flourish subhead
</commit_message>
<xml_diff>
--- a/Processed Data/Subject Demographics_Mental Health Flag_TRRs.xlsx
+++ b/Processed Data/Subject Demographics_Mental Health Flag_TRRs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MaggieDougherty/Documents/GitHub/CPD-Mental-Health/Processed Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D8A17D-611D-344D-9CBB-81FBC35F7AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518C1BBA-B451-F141-8BD5-663198A8CFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24880" windowHeight="14040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3220" yWindow="500" windowWidth="22380" windowHeight="14040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>WARD</t>
   </si>
@@ -70,23 +70,29 @@
     <t>TOTAL INCIDENTS</t>
   </si>
   <si>
-    <t>SubjRace: Black</t>
+    <t>Black</t>
   </si>
   <si>
-    <t>SubjRace: White</t>
+    <t>White</t>
   </si>
   <si>
-    <t>SubjRace: Hispanic</t>
+    <t>Hispanic</t>
   </si>
   <si>
-    <t>SubjRace: Other</t>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Raw Data</t>
+  </si>
+  <si>
+    <t>Percentages</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +102,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,17 +133,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2131,1296 +2152,2335 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FBB90E-BA38-664E-A711-351211E64410}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="28.83203125" customWidth="1"/>
-    <col min="9" max="9" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="H2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <f>SUM(Sheet1!B2:J2)</f>
         <v>36</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <f>Sheet1!B2</f>
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <f>Sheet1!E2</f>
         <v>9</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <f>Sheet1!C2+Sheet1!F2</f>
         <v>11</v>
       </c>
-      <c r="F2">
-        <f>B2-SUM(C2:E2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="F3">
+        <f>B3-SUM(C3:E3)</f>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <f>C3/$B3</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:L3" si="0">D3/$B3</f>
+        <v>0.25</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" si="0"/>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <f>SUM(Sheet1!B3:J3)</f>
         <v>61</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <f>Sheet1!B3</f>
         <v>26</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <f>Sheet1!E3</f>
         <v>31</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <f>Sheet1!C3+Sheet1!F3</f>
         <v>4</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F51" si="0">B3-SUM(C3:E3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="F4">
+        <f t="shared" ref="F4:F52" si="1">B4-SUM(C4:E4)</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I52" si="2">C4/$B4</f>
+        <v>0.42622950819672129</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J52" si="3">D4/$B4</f>
+        <v>0.50819672131147542</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ref="K4:K52" si="4">E4/$B4</f>
+        <v>6.5573770491803282E-2</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:L52" si="5">F4/$B4</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <f>SUM(Sheet1!B4:J4)</f>
         <v>78</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <f>Sheet1!B4</f>
         <v>60</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <f>Sheet1!E4</f>
         <v>8</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <f>Sheet1!C4+Sheet1!F4</f>
         <v>5</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
+      <c r="F5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="2"/>
+        <v>0.76923076923076927</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="3"/>
+        <v>0.10256410256410256</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="4"/>
+        <v>6.4102564102564097E-2</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="5"/>
+        <v>6.4102564102564097E-2</v>
+      </c>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <f>SUM(Sheet1!B5:J5)</f>
         <v>48</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <f>Sheet1!B5</f>
         <v>43</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <f>Sheet1!E5</f>
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <f>Sheet1!C5+Sheet1!F5</f>
         <v>0</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="5"/>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f>SUM(Sheet1!B6:J6)</f>
         <v>60</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <f>Sheet1!B6</f>
         <v>57</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <f>Sheet1!E6</f>
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <f>Sheet1!C6+Sheet1!F6</f>
         <v>3</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="4"/>
+        <v>0.05</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <f>SUM(Sheet1!B7:J7)</f>
         <v>114</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <f>Sheet1!B7</f>
         <v>113</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <f>Sheet1!E7</f>
         <v>0</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <f>Sheet1!C7+Sheet1!F7</f>
         <v>0</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.99122807017543857</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="5"/>
+        <v>8.771929824561403E-3</v>
+      </c>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <f>SUM(Sheet1!B8:J8)</f>
         <v>79</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <f>Sheet1!B8</f>
         <v>76</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <f>Sheet1!E8</f>
         <v>0</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <f>Sheet1!C8+Sheet1!F8</f>
         <v>0</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
+      <c r="F9">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.96202531645569622</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="5"/>
+        <v>3.7974683544303799E-2</v>
+      </c>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <f>SUM(Sheet1!B9:J9)</f>
         <v>102</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <f>Sheet1!B9</f>
         <v>99</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <f>Sheet1!E9</f>
         <v>1</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <f>Sheet1!C9+Sheet1!F9</f>
         <v>1</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.97058823529411764</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="3"/>
+        <v>9.8039215686274508E-3</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="4"/>
+        <v>9.8039215686274508E-3</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="5"/>
+        <v>9.8039215686274508E-3</v>
+      </c>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <f>SUM(Sheet1!B10:J10)</f>
         <v>68</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <f>Sheet1!B10</f>
         <v>58</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <f>Sheet1!E10</f>
         <v>6</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <f>Sheet1!C10+Sheet1!F10</f>
         <v>4</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.8529411764705882</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="3"/>
+        <v>8.8235294117647065E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="4"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <f>SUM(Sheet1!B11:J11)</f>
         <v>35</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <f>Sheet1!B11</f>
         <v>9</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <f>Sheet1!E11</f>
         <v>7</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <f>Sheet1!C11+Sheet1!F11</f>
         <v>17</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
+      <c r="F12">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.25714285714285712</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="4"/>
+        <v>0.48571428571428571</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="5"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <f>SUM(Sheet1!B12:J12)</f>
         <v>12</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <f>Sheet1!B12</f>
         <v>6</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <f>Sheet1!E12</f>
         <v>4</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <f>Sheet1!C12+Sheet1!F12</f>
         <v>2</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <f>SUM(Sheet1!B13:J13)</f>
         <v>21</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <f>Sheet1!B13</f>
         <v>2</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <f>Sheet1!E13</f>
         <v>5</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <f>Sheet1!C13+Sheet1!F13</f>
         <v>14</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="2"/>
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="3"/>
+        <v>0.23809523809523808</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="4"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <f>SUM(Sheet1!B14:J14)</f>
         <v>21</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <f>Sheet1!B14</f>
         <v>8</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <f>Sheet1!E14</f>
         <v>6</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <f>Sheet1!C14+Sheet1!F14</f>
         <v>7</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="2"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="3"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <f>SUM(Sheet1!B15:J15)</f>
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <f>Sheet1!B15</f>
         <v>4</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <f>Sheet1!E15</f>
         <v>3</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <f>Sheet1!C15+Sheet1!F15</f>
         <v>7</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="2"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="3"/>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <f>SUM(Sheet1!B16:J16)</f>
         <v>42</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <f>Sheet1!B16</f>
         <v>19</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <f>Sheet1!E16</f>
         <v>3</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <f>Sheet1!C16+Sheet1!F16</f>
         <v>19</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="2"/>
+        <v>0.45238095238095238</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="3"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="4"/>
+        <v>0.45238095238095238</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="5"/>
+        <v>2.3809523809523808E-2</v>
+      </c>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <f>SUM(Sheet1!B17:J17)</f>
         <v>84</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <f>Sheet1!B17</f>
         <v>78</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <f>Sheet1!E17</f>
         <v>0</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <f>Sheet1!C17+Sheet1!F17</f>
         <v>4</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
+      <c r="F18">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="H18">
+        <v>16</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="2"/>
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="4"/>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="5"/>
+        <v>2.3809523809523808E-2</v>
+      </c>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <f>SUM(Sheet1!B18:J18)</f>
         <v>88</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <f>Sheet1!B18</f>
         <v>76</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <f>Sheet1!E18</f>
         <v>1</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <f>Sheet1!C18+Sheet1!F18</f>
         <v>11</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>17</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="2"/>
+        <v>0.86363636363636365</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="3"/>
+        <v>1.1363636363636364E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <f>SUM(Sheet1!B19:J19)</f>
         <v>22</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <f>Sheet1!B19</f>
         <v>15</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <f>Sheet1!E19</f>
         <v>6</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <f>Sheet1!C19+Sheet1!F19</f>
         <v>1</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="2"/>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="3"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="4"/>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <f>SUM(Sheet1!B20:J20)</f>
         <v>20</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <f>Sheet1!B20</f>
         <v>17</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <f>Sheet1!E20</f>
         <v>2</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <f>Sheet1!C20+Sheet1!F20</f>
         <v>1</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>19</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="2"/>
+        <v>0.85</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="4"/>
+        <v>0.05</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <f>SUM(Sheet1!B21:J21)</f>
         <v>111</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <f>Sheet1!B21</f>
         <v>107</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <f>Sheet1!E21</f>
         <v>0</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <f>Sheet1!C21+Sheet1!F21</f>
         <v>4</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>20</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="2"/>
+        <v>0.963963963963964</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="4"/>
+        <v>3.6036036036036036E-2</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <f>SUM(Sheet1!B22:J22)</f>
         <v>88</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <f>Sheet1!B22</f>
         <v>88</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <f>Sheet1!E22</f>
         <v>0</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <f>Sheet1!C22+Sheet1!F22</f>
         <v>0</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>21</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <f>SUM(Sheet1!B23:J23)</f>
         <v>20</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <f>Sheet1!B23</f>
         <v>6</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <f>Sheet1!E23</f>
         <v>2</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <f>Sheet1!C23+Sheet1!F23</f>
         <v>12</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>22</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="4"/>
+        <v>0.6</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <f>SUM(Sheet1!B24:J24)</f>
         <v>11</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <f>Sheet1!B24</f>
         <v>2</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <f>Sheet1!E24</f>
         <v>2</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <f>Sheet1!C24+Sheet1!F24</f>
         <v>7</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>23</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="2"/>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="3"/>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="4"/>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <f>SUM(Sheet1!B25:J25)</f>
         <v>167</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <f>Sheet1!B25</f>
         <v>142</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <f>Sheet1!E25</f>
         <v>4</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <f>Sheet1!C25+Sheet1!F25</f>
         <v>20</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>24</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="2"/>
+        <v>0.85029940119760483</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="3"/>
+        <v>2.3952095808383235E-2</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="4"/>
+        <v>0.11976047904191617</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="5"/>
+        <v>5.9880239520958087E-3</v>
+      </c>
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <f>SUM(Sheet1!B26:J26)</f>
         <v>32</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <f>Sheet1!B26</f>
         <v>12</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <f>Sheet1!E26</f>
         <v>2</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <f>Sheet1!C26+Sheet1!F26</f>
         <v>18</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>25</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="2"/>
+        <v>0.375</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="3"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="4"/>
+        <v>0.5625</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <f>SUM(Sheet1!B27:J27)</f>
         <v>30</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <f>Sheet1!B27</f>
         <v>5</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <f>Sheet1!E27</f>
         <v>3</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <f>Sheet1!C27+Sheet1!F27</f>
         <v>22</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>26</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="4"/>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="3"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <f>SUM(Sheet1!B28:J28)</f>
         <v>103</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <f>Sheet1!B28</f>
         <v>71</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <f>Sheet1!E28</f>
         <v>23</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <f>Sheet1!C28+Sheet1!F28</f>
         <v>7</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="0"/>
+      <c r="F29">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="H29">
+        <v>27</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="2"/>
+        <v>0.68932038834951459</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="3"/>
+        <v>0.22330097087378642</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="4"/>
+        <v>6.7961165048543687E-2</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="5"/>
+        <v>1.9417475728155338E-2</v>
+      </c>
+      <c r="N29" s="3"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <f>SUM(Sheet1!B29:J29)</f>
         <v>124</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <f>Sheet1!B29</f>
         <v>119</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <f>Sheet1!E29</f>
         <v>2</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <f>Sheet1!C29+Sheet1!F29</f>
         <v>3</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>28</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="2"/>
+        <v>0.95967741935483875</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="3"/>
+        <v>1.6129032258064516E-2</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="4"/>
+        <v>2.4193548387096774E-2</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="3"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <f>SUM(Sheet1!B30:J30)</f>
         <v>86</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <f>Sheet1!B30</f>
         <v>78</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <f>Sheet1!E30</f>
         <v>2</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <f>Sheet1!C30+Sheet1!F30</f>
         <v>5</v>
       </c>
-      <c r="F30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>29</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="2"/>
+        <v>0.90697674418604646</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="3"/>
+        <v>2.3255813953488372E-2</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="4"/>
+        <v>5.8139534883720929E-2</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="5"/>
+        <v>1.1627906976744186E-2</v>
+      </c>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <f>SUM(Sheet1!B31:J31)</f>
         <v>43</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <f>Sheet1!B31</f>
         <v>13</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <f>Sheet1!E31</f>
         <v>6</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <f>Sheet1!C31+Sheet1!F31</f>
         <v>24</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>30</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="2"/>
+        <v>0.30232558139534882</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13953488372093023</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="4"/>
+        <v>0.55813953488372092</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="3"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <f>SUM(Sheet1!B32:J32)</f>
         <v>26</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <f>Sheet1!B32</f>
         <v>5</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <f>Sheet1!E32</f>
         <v>7</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <f>Sheet1!C32+Sheet1!F32</f>
         <v>14</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>31</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="2"/>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26923076923076922</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="4"/>
+        <v>0.53846153846153844</v>
+      </c>
+      <c r="L33" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="3"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <f>SUM(Sheet1!B33:J33)</f>
         <v>10</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <f>Sheet1!B33</f>
         <v>0</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <f>Sheet1!E33</f>
         <v>6</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <f>Sheet1!C33+Sheet1!F33</f>
         <v>4</v>
       </c>
-      <c r="F33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>32</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="4"/>
+        <v>0.4</v>
+      </c>
+      <c r="L34" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="3"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <f>SUM(Sheet1!B34:J34)</f>
         <v>39</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <f>Sheet1!B34</f>
         <v>11</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <f>Sheet1!E34</f>
         <v>14</v>
       </c>
-      <c r="E34">
+      <c r="E35">
         <f>Sheet1!C34+Sheet1!F34</f>
         <v>7</v>
       </c>
-      <c r="F34">
-        <f t="shared" si="0"/>
+      <c r="F35">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="H35">
+        <v>33</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="2"/>
+        <v>0.28205128205128205</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="3"/>
+        <v>0.35897435897435898</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" si="4"/>
+        <v>0.17948717948717949</v>
+      </c>
+      <c r="L35" s="2">
+        <f t="shared" si="5"/>
+        <v>0.17948717948717949</v>
+      </c>
+      <c r="N35" s="3"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>34</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <f>SUM(Sheet1!B35:J35)</f>
         <v>55</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <f>Sheet1!B35</f>
         <v>44</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <f>Sheet1!E35</f>
         <v>9</v>
       </c>
-      <c r="E35">
+      <c r="E36">
         <f>Sheet1!C35+Sheet1!F35</f>
         <v>1</v>
       </c>
-      <c r="F35">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>34</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="3"/>
+        <v>0.16363636363636364</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="4"/>
+        <v>1.8181818181818181E-2</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="5"/>
+        <v>1.8181818181818181E-2</v>
+      </c>
+      <c r="N36" s="3"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37">
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <f>SUM(Sheet1!B36:J36)</f>
         <v>37</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <f>Sheet1!B36</f>
         <v>4</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <f>Sheet1!E36</f>
         <v>9</v>
       </c>
-      <c r="E36">
+      <c r="E37">
         <f>Sheet1!C36+Sheet1!F36</f>
         <v>24</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>35</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="2"/>
+        <v>0.10810810810810811</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24324324324324326</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="4"/>
+        <v>0.64864864864864868</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N37" s="3"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <f>SUM(Sheet1!B37:J37)</f>
         <v>32</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <f>Sheet1!B37</f>
         <v>10</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <f>Sheet1!E37</f>
         <v>6</v>
       </c>
-      <c r="E37">
+      <c r="E38">
         <f>Sheet1!C37+Sheet1!F37</f>
         <v>15</v>
       </c>
-      <c r="F37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>36</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="2"/>
+        <v>0.3125</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1875</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="4"/>
+        <v>0.46875</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="5"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="N38" s="3"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <f>SUM(Sheet1!B38:J38)</f>
         <v>107</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <f>Sheet1!B38</f>
         <v>77</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <f>Sheet1!E38</f>
         <v>8</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <f>Sheet1!C38+Sheet1!F38</f>
         <v>21</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>37</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="2"/>
+        <v>0.71962616822429903</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="3"/>
+        <v>7.476635514018691E-2</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="4"/>
+        <v>0.19626168224299065</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="5"/>
+        <v>9.3457943925233638E-3</v>
+      </c>
+      <c r="N39" s="3"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>38</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <f>SUM(Sheet1!B39:J39)</f>
         <v>15</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <f>Sheet1!B39</f>
         <v>0</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <f>Sheet1!E39</f>
         <v>9</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <f>Sheet1!C39+Sheet1!F39</f>
         <v>4</v>
       </c>
-      <c r="F39">
-        <f t="shared" si="0"/>
+      <c r="F40">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="H40">
+        <v>38</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="4"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="5"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="N40" s="3"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>39</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <f>SUM(Sheet1!B40:J40)</f>
         <v>45</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <f>Sheet1!B40</f>
         <v>13</v>
       </c>
-      <c r="D40">
+      <c r="D41">
         <f>Sheet1!E40</f>
         <v>23</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <f>Sheet1!C40+Sheet1!F40</f>
         <v>9</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>39</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="2"/>
+        <v>0.28888888888888886</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="3"/>
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N41" s="3"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <f>SUM(Sheet1!B41:J41)</f>
         <v>44</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <f>Sheet1!B41</f>
         <v>16</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <f>Sheet1!E41</f>
         <v>12</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <f>Sheet1!C41+Sheet1!F41</f>
         <v>14</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="0"/>
+      <c r="F42">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="H42">
+        <v>40</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="2"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="3"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="K42" s="2">
+        <f t="shared" si="4"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="L42" s="2">
+        <f t="shared" si="5"/>
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="N42" s="3"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43">
         <v>41</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <f>SUM(Sheet1!B42:J42)</f>
         <v>84</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <f>Sheet1!B42</f>
         <v>34</v>
       </c>
-      <c r="D42">
+      <c r="D43">
         <f>Sheet1!E42</f>
         <v>38</v>
       </c>
-      <c r="E42">
+      <c r="E43">
         <f>Sheet1!C42+Sheet1!F42</f>
         <v>9</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="0"/>
+      <c r="F43">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="H43">
+        <v>41</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="2"/>
+        <v>0.40476190476190477</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="3"/>
+        <v>0.45238095238095238</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" si="4"/>
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="L43" s="2">
+        <f t="shared" si="5"/>
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="N43" s="3"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44">
         <v>42</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <f>SUM(Sheet1!B43:J43)</f>
         <v>81</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <f>Sheet1!B43</f>
         <v>60</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <f>Sheet1!E43</f>
         <v>13</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <f>Sheet1!C43+Sheet1!F43</f>
         <v>7</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>42</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="2"/>
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="3"/>
+        <v>0.16049382716049382</v>
+      </c>
+      <c r="K44" s="2">
+        <f t="shared" si="4"/>
+        <v>8.6419753086419748E-2</v>
+      </c>
+      <c r="L44" s="2">
+        <f t="shared" si="5"/>
+        <v>1.2345679012345678E-2</v>
+      </c>
+      <c r="N44" s="3"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45">
         <v>43</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <f>SUM(Sheet1!B44:J44)</f>
         <v>16</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <f>Sheet1!B44</f>
         <v>9</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <f>Sheet1!E44</f>
         <v>4</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <f>Sheet1!C44+Sheet1!F44</f>
         <v>1</v>
       </c>
-      <c r="F44">
-        <f t="shared" si="0"/>
+      <c r="F45">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="H45">
+        <v>43</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5625</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="K45" s="2">
+        <f t="shared" si="4"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="L45" s="2">
+        <f t="shared" si="5"/>
+        <v>0.125</v>
+      </c>
+      <c r="N45" s="3"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46">
         <v>44</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <f>SUM(Sheet1!B45:J45)</f>
         <v>57</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <f>Sheet1!B45</f>
         <v>25</v>
       </c>
-      <c r="D45">
+      <c r="D46">
         <f>Sheet1!E45</f>
         <v>23</v>
       </c>
-      <c r="E45">
+      <c r="E46">
         <f>Sheet1!C45+Sheet1!F45</f>
         <v>8</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>44</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="2"/>
+        <v>0.43859649122807015</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="3"/>
+        <v>0.40350877192982454</v>
+      </c>
+      <c r="K46" s="2">
+        <f t="shared" si="4"/>
+        <v>0.14035087719298245</v>
+      </c>
+      <c r="L46" s="2">
+        <f t="shared" si="5"/>
+        <v>1.7543859649122806E-2</v>
+      </c>
+      <c r="N46" s="3"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47">
         <v>45</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <f>SUM(Sheet1!B46:J46)</f>
         <v>28</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <f>Sheet1!B46</f>
         <v>7</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <f>Sheet1!E46</f>
         <v>15</v>
       </c>
-      <c r="E46">
+      <c r="E47">
         <f>Sheet1!C46+Sheet1!F46</f>
         <v>4</v>
       </c>
-      <c r="F46">
-        <f t="shared" si="0"/>
+      <c r="F47">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="H47">
+        <v>45</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="J47" s="2">
+        <f t="shared" si="3"/>
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="K47" s="2">
+        <f t="shared" si="4"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="L47" s="2">
+        <f t="shared" si="5"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="N47" s="3"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48">
         <v>46</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <f>SUM(Sheet1!B47:J47)</f>
         <v>99</v>
       </c>
-      <c r="C47">
+      <c r="C48">
         <f>Sheet1!B47</f>
         <v>52</v>
       </c>
-      <c r="D47">
+      <c r="D48">
         <f>Sheet1!E47</f>
         <v>28</v>
       </c>
-      <c r="E47">
+      <c r="E48">
         <f>Sheet1!C47+Sheet1!F47</f>
         <v>19</v>
       </c>
-      <c r="F47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>46</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5252525252525253</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="3"/>
+        <v>0.28282828282828282</v>
+      </c>
+      <c r="K48" s="2">
+        <f t="shared" si="4"/>
+        <v>0.19191919191919191</v>
+      </c>
+      <c r="L48" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N48" s="3"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49">
         <v>47</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <f>SUM(Sheet1!B48:J48)</f>
         <v>31</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <f>Sheet1!B48</f>
         <v>16</v>
       </c>
-      <c r="D48">
+      <c r="D49">
         <f>Sheet1!E48</f>
         <v>11</v>
       </c>
-      <c r="E48">
+      <c r="E49">
         <f>Sheet1!C48+Sheet1!F48</f>
         <v>3</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>47</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5161290322580645</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" si="3"/>
+        <v>0.35483870967741937</v>
+      </c>
+      <c r="K49" s="2">
+        <f t="shared" si="4"/>
+        <v>9.6774193548387094E-2</v>
+      </c>
+      <c r="L49" s="2">
+        <f t="shared" si="5"/>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="N49" s="3"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50">
         <v>48</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <f>SUM(Sheet1!B49:J49)</f>
         <v>58</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <f>Sheet1!B49</f>
         <v>37</v>
       </c>
-      <c r="D49">
+      <c r="D50">
         <f>Sheet1!E49</f>
         <v>13</v>
       </c>
-      <c r="E49">
+      <c r="E50">
         <f>Sheet1!C49+Sheet1!F49</f>
         <v>4</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="0"/>
+      <c r="F50">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="H50">
+        <v>48</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="2"/>
+        <v>0.63793103448275867</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" si="3"/>
+        <v>0.22413793103448276</v>
+      </c>
+      <c r="K50" s="2">
+        <f t="shared" si="4"/>
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="L50" s="2">
+        <f t="shared" si="5"/>
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="N50" s="3"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51">
         <v>49</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <f>SUM(Sheet1!B50:J50)</f>
         <v>62</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <f>Sheet1!B50</f>
         <v>38</v>
       </c>
-      <c r="D50">
+      <c r="D51">
         <f>Sheet1!E50</f>
         <v>12</v>
       </c>
-      <c r="E50">
+      <c r="E51">
         <f>Sheet1!C50+Sheet1!F50</f>
         <v>11</v>
       </c>
-      <c r="F50">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>49</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="2"/>
+        <v>0.61290322580645162</v>
+      </c>
+      <c r="J51" s="2">
+        <f t="shared" si="3"/>
+        <v>0.19354838709677419</v>
+      </c>
+      <c r="K51" s="2">
+        <f t="shared" si="4"/>
+        <v>0.17741935483870969</v>
+      </c>
+      <c r="L51" s="2">
+        <f t="shared" si="5"/>
+        <v>1.6129032258064516E-2</v>
+      </c>
+      <c r="N51" s="3"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52">
         <v>50</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <f>SUM(Sheet1!B51:J51)</f>
         <v>26</v>
       </c>
-      <c r="C51">
+      <c r="C52">
         <f>Sheet1!B51</f>
         <v>8</v>
       </c>
-      <c r="D51">
+      <c r="D52">
         <f>Sheet1!E51</f>
         <v>10</v>
       </c>
-      <c r="E51">
+      <c r="E52">
         <f>Sheet1!C51+Sheet1!F51</f>
         <v>3</v>
       </c>
-      <c r="F51">
-        <f t="shared" si="0"/>
+      <c r="F52">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="H52">
+        <v>50</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="2"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="J52" s="2">
+        <f t="shared" si="3"/>
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="K52" s="2">
+        <f t="shared" si="4"/>
+        <v>0.11538461538461539</v>
+      </c>
+      <c r="L52" s="2">
+        <f t="shared" si="5"/>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="N52" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>